<commit_message>
Concluded the research graph
</commit_message>
<xml_diff>
--- a/OSS Projects.xlsx
+++ b/OSS Projects.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="8865" tabRatio="660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="8865" tabRatio="660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Software Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Orange Tests" sheetId="13" r:id="rId2"/>
-    <sheet name="Yellow Tests" sheetId="2" r:id="rId3"/>
-    <sheet name="Red Tests" sheetId="8" r:id="rId4"/>
-    <sheet name="Green Tests" sheetId="9" r:id="rId5"/>
-    <sheet name="Blue Tests" sheetId="10" r:id="rId6"/>
-    <sheet name="Purple Tests" sheetId="11" r:id="rId7"/>
+    <sheet name="Full Graphs" sheetId="14" r:id="rId2"/>
+    <sheet name="Orange Tests" sheetId="13" r:id="rId3"/>
+    <sheet name="Yellow Tests" sheetId="2" r:id="rId4"/>
+    <sheet name="Red Tests" sheetId="8" r:id="rId5"/>
+    <sheet name="Green Tests" sheetId="9" r:id="rId6"/>
+    <sheet name="Blue Tests" sheetId="10" r:id="rId7"/>
+    <sheet name="Purple Tests" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -293,13 +294,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF9933FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9933FF"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -470,31 +471,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -503,12 +489,99 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -742,21 +815,2412 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Maintainability Index</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>86.784440842787689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.286523929471031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.423739732646155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.032802608862454</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>85.58</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>84.33</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>83.94</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>85.14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80.018543262180216</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.158812809164274</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.075117370892016</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.309096837300288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="20820352"/>
+        <c:axId val="20822272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="20820352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="20822272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="20822272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="20820352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Cyclomatic Complexity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.740140464613722</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6428211586901762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0171686261877921</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4992518703241897</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>8.66</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>8.48</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>6.92</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>9.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8712726087664979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6638896120801876</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5712050078247257</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.041082491033583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="212378368"/>
+        <c:axId val="212379904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="212378368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="212379904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="212379904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="212378368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Depth of Inheritance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.4701492537313432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2278702892199824</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7772756617172369</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9275538041830858</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3866023275617372</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4705882352941178</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6370967741935485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="21344640"/>
+        <c:axId val="212224640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="21344640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="212224640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="212224640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="21344640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Class Coupling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$E$2:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.9497568881685572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6474811083123422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8153970043485259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9874544408210246</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>5.52</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.6100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1071533322470266</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7330556278746858</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7766040688575897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.7401369416367789</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="217071616"/>
+        <c:axId val="217073152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="217071616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="217073152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="217073152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="217071616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Average Weekly Commits</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="217158016"/>
+        <c:axId val="217159936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="217158016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="217159936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="217159936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="217158016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Commits Per Contributor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9933FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Graphs'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>nopCommerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AutoFixture-master</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>smartstoreag</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Glimpse-master</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ATF-master</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OptiKey-master</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PokemonGo-Bot-master</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CodeHub-master</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duplicati-master</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mongo-csharp-driver-master</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SignalR-dev</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ImageProcessor-develop</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Hearthstone-Deck-Tracker-master</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Graphs'!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>302.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>574.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81.180000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="212120704"/>
+        <c:axId val="214700800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="212120704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="214700800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="214700800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="212120704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:H14"/>
   <sortState ref="A2:H14">
     <sortCondition descending="1" ref="B1:B14"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" name="Size (mB)" dataDxfId="6"/>
-    <tableColumn id="3" name="Folders" dataDxfId="5"/>
-    <tableColumn id="4" name="Files" dataDxfId="4"/>
-    <tableColumn id="5" name="Percent of C#" dataDxfId="3"/>
-    <tableColumn id="6" name="GitHub Stars" dataDxfId="2"/>
-    <tableColumn id="7" name="Brief Description" dataDxfId="1"/>
-    <tableColumn id="8" name="Link" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" name="Size (mB)" dataDxfId="10"/>
+    <tableColumn id="3" name="Folders" dataDxfId="9"/>
+    <tableColumn id="4" name="Files" dataDxfId="8"/>
+    <tableColumn id="5" name="Percent of C#" dataDxfId="7"/>
+    <tableColumn id="6" name="GitHub Stars" dataDxfId="6"/>
+    <tableColumn id="7" name="Brief Description" dataDxfId="5"/>
+    <tableColumn id="8" name="Link" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:G14"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Maintainability Index"/>
+    <tableColumn id="3" name="Cyclomatic Complexity"/>
+    <tableColumn id="4" name="Depth of Inheritance"/>
+    <tableColumn id="5" name="Class Coupling"/>
+    <tableColumn id="6" name="Average Weekly Commits"/>
+    <tableColumn id="7" name="Commits Per Contributor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1017,7 +3481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1028,7 +3492,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,80 +3533,80 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="62">
         <v>101</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="60">
         <v>4313</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="60">
         <v>766</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="61">
         <v>85.4</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="60">
         <v>1456</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="63" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="64">
         <v>101</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="59">
         <v>1521</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="59">
         <v>219</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="55">
         <v>98.1</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="59">
         <v>1109</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="63" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="62">
         <v>98</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="60">
         <v>5262</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="60">
         <v>857</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="61">
         <v>85.1</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="60">
         <v>841</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="66" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1168,7 +3632,7 @@
       <c r="G5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="30" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1303,106 +3767,106 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="38">
         <v>35.700000000000003</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="39">
         <v>3309</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="39">
         <v>334</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="37">
         <v>97.5</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="39">
         <v>1603</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="40" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="38">
         <v>29.4</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="39">
         <v>1342</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="39">
         <v>258</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="37">
         <v>82.7</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="39">
         <v>6551</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="40" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="34">
         <v>24.7</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="35">
         <v>479</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="35">
         <v>127</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="33">
         <v>97.2</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="35">
         <v>1650</v>
       </c>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="36" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="34">
         <v>21.1</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="35">
         <v>3301</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="35">
         <v>104</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="33">
         <v>99.7</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="35">
         <v>2917</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1477,10 +3941,360 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="56">
+        <v>86.784440842787689</v>
+      </c>
+      <c r="C2" s="56">
+        <v>6.740140464613722</v>
+      </c>
+      <c r="D2" s="56">
+        <v>2.4701492537313432</v>
+      </c>
+      <c r="E2" s="56">
+        <v>5.9497568881685572</v>
+      </c>
+      <c r="F2" s="57">
+        <v>20.03</v>
+      </c>
+      <c r="G2" s="58">
+        <v>302.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="56">
+        <v>81.286523929471031</v>
+      </c>
+      <c r="C3" s="56">
+        <v>5.6428211586901762</v>
+      </c>
+      <c r="D3" s="56">
+        <v>1.2278702892199824</v>
+      </c>
+      <c r="E3" s="56">
+        <v>6.6474811083123422</v>
+      </c>
+      <c r="F3" s="57">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="G3" s="58">
+        <v>64.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="56">
+        <v>87.423739732646155</v>
+      </c>
+      <c r="C4" s="56">
+        <v>7.0171686261877921</v>
+      </c>
+      <c r="D4" s="56">
+        <v>1.7772756617172369</v>
+      </c>
+      <c r="E4" s="56">
+        <v>4.8153970043485259</v>
+      </c>
+      <c r="F4" s="57">
+        <v>20.88</v>
+      </c>
+      <c r="G4" s="58">
+        <v>574.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27">
+        <v>89.32</v>
+      </c>
+      <c r="C5" s="27">
+        <v>5.72</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="E5" s="27">
+        <v>3.85</v>
+      </c>
+      <c r="F5" s="21">
+        <v>7.7</v>
+      </c>
+      <c r="G5" s="46">
+        <v>57.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="27">
+        <v>83.032802608862454</v>
+      </c>
+      <c r="C6" s="27">
+        <v>7.4992518703241897</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1.9275538041830858</v>
+      </c>
+      <c r="E6" s="27">
+        <v>4.9874544408210246</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0.89</v>
+      </c>
+      <c r="G6" s="46">
+        <v>22.71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="22">
+        <v>85.58</v>
+      </c>
+      <c r="C7" s="22">
+        <v>8.66</v>
+      </c>
+      <c r="D7" s="22">
+        <v>3.61</v>
+      </c>
+      <c r="E7" s="22">
+        <v>5.52</v>
+      </c>
+      <c r="F7" s="22">
+        <v>12.33</v>
+      </c>
+      <c r="G7" s="47">
+        <v>61.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="22">
+        <v>84.33</v>
+      </c>
+      <c r="C8" s="22">
+        <v>8.48</v>
+      </c>
+      <c r="D8" s="22">
+        <v>1.25</v>
+      </c>
+      <c r="E8" s="22">
+        <v>3.49</v>
+      </c>
+      <c r="F8" s="22">
+        <v>19.66</v>
+      </c>
+      <c r="G8" s="47">
+        <v>36.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="23">
+        <v>83.94</v>
+      </c>
+      <c r="C9" s="23">
+        <v>6.92</v>
+      </c>
+      <c r="D9" s="23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E9" s="23">
+        <v>6.8</v>
+      </c>
+      <c r="F9" s="23">
+        <v>2.48</v>
+      </c>
+      <c r="G9" s="48">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="23">
+        <v>85.14</v>
+      </c>
+      <c r="C10" s="23">
+        <v>9.08</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1.18</v>
+      </c>
+      <c r="E10" s="23">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="F10" s="23">
+        <v>9.27</v>
+      </c>
+      <c r="G10" s="48">
+        <v>81.180000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25">
+        <v>80.018543262180216</v>
+      </c>
+      <c r="C11" s="25">
+        <v>5.8712726087664979</v>
+      </c>
+      <c r="D11" s="25">
+        <v>1.3866023275617372</v>
+      </c>
+      <c r="E11" s="25">
+        <v>7.1071533322470266</v>
+      </c>
+      <c r="F11" s="24">
+        <v>8.17</v>
+      </c>
+      <c r="G11" s="49">
+        <v>72.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25">
+        <v>83.158812809164274</v>
+      </c>
+      <c r="C12" s="25">
+        <v>6.6638896120801876</v>
+      </c>
+      <c r="D12" s="25">
+        <v>1.4705882352941178</v>
+      </c>
+      <c r="E12" s="25">
+        <v>5.7330556278746858</v>
+      </c>
+      <c r="F12" s="24">
+        <v>14.75</v>
+      </c>
+      <c r="G12" s="49">
+        <v>61.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="32">
+        <v>83.075117370892016</v>
+      </c>
+      <c r="C13" s="32">
+        <v>6.5712050078247257</v>
+      </c>
+      <c r="D13" s="32">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="E13" s="32">
+        <v>4.7766040688575897</v>
+      </c>
+      <c r="F13" s="31">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G13" s="50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="52">
+        <v>84.309096837300288</v>
+      </c>
+      <c r="C14" s="52">
+        <v>8.041082491033583</v>
+      </c>
+      <c r="D14" s="52">
+        <v>2.6370967741935485</v>
+      </c>
+      <c r="E14" s="52">
+        <v>4.7401369416367789</v>
+      </c>
+      <c r="F14" s="53">
+        <v>19.2</v>
+      </c>
+      <c r="G14" s="54">
+        <v>40.93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,159 +4302,159 @@
     <col min="1" max="1" width="22.7109375" style="28" customWidth="1"/>
     <col min="2" max="6" width="15.7109375" style="28" customWidth="1"/>
     <col min="7" max="11" width="23.7109375" style="28" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" style="34" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="29" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="59">
         <v>101</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="59">
         <v>4313</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="59">
         <v>766</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="59">
         <v>85.4</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="59">
         <v>1456</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="56">
         <v>86.784440842787689</v>
       </c>
-      <c r="H2" s="33">
+      <c r="H2" s="56">
         <v>6.740140464613722</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="56">
         <v>2.4701492537313432</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="56">
         <v>5.9497568881685572</v>
       </c>
-      <c r="K2" s="32">
+      <c r="K2" s="57">
         <v>20.03</v>
       </c>
-      <c r="L2" s="32">
+      <c r="L2" s="57">
         <v>302.57</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="59">
         <v>101</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="59">
         <v>1521</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="59">
         <v>219</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="59">
         <v>98.1</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="59">
         <v>1109</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="56">
         <v>81.286523929471031</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="56">
         <v>5.6428211586901762</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="56">
         <v>1.2278702892199824</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="56">
         <v>6.6474811083123422</v>
       </c>
-      <c r="K3" s="32">
+      <c r="K3" s="57">
         <v>8.7200000000000006</v>
       </c>
-      <c r="L3" s="32">
+      <c r="L3" s="57">
         <v>64.78</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="59">
         <v>98</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="59">
         <v>5262</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="59">
         <v>857</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="59">
         <v>85.1</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="59">
         <v>841</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="56">
         <v>87.423739732646155</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="56">
         <v>7.0171686261877921</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="56">
         <v>1.7772756617172369</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="56">
         <v>4.8153970043485259</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="57">
         <v>20.88</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="57">
         <v>574.62</v>
       </c>
     </row>
@@ -1650,12 +4464,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +4594,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="34"/>
+      <c r="L4" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1788,12 +4602,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,12 +4737,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,12 +4872,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,17 +5007,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="12" width="23.7109375" customWidth="1"/>
   </cols>
@@ -2247,78 +5061,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="31">
         <v>24.7</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="31">
         <v>479</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="31">
         <v>127</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="31">
         <v>97.2</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="31">
         <v>1650</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="32">
         <v>83.075117370892016</v>
       </c>
-      <c r="H2" s="43">
+      <c r="H2" s="32">
         <v>6.5712050078247257</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="32">
         <v>1.2450000000000001</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="32">
         <v>4.7766040688575897</v>
       </c>
-      <c r="K2" s="42">
+      <c r="K2" s="31">
         <v>8.4600000000000009</v>
       </c>
-      <c r="L2" s="42">
+      <c r="L2" s="31">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="31">
         <v>21.1</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="31">
         <v>3301</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="31">
         <v>104</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="31">
         <v>99.7</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="31">
         <v>2917</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="32">
         <v>84.309096837300288</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="32">
         <v>8.041082491033583</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="32">
         <v>2.6370967741935485</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="32">
         <v>4.7401369416367789</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="31">
         <v>19.2</v>
       </c>
-      <c r="L3" s="42">
+      <c r="L3" s="31">
         <v>40.93</v>
       </c>
     </row>

</xml_diff>